<commit_message>
version of final export
</commit_message>
<xml_diff>
--- a/templates/packlista_template.xlsx
+++ b/templates/packlista_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\Jupyter\Enterprise\SvenskaKyrkan\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E67FF5-B5D5-4BEE-8A96-DE76A044C55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0513B83-B9EA-44CB-B199-5F3343279126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -526,6 +526,9 @@
     </xf>
     <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,9 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,31 +870,31 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="36" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" style="36" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" style="36" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="36" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="36" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="36" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" style="36" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="36" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="36" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" style="36" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="36" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="36" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="36" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="36" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="36" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="36" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33"/>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
@@ -902,31 +902,31 @@
         <v>22</v>
       </c>
       <c r="G1" s="38"/>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="48"/>
+      <c r="I1" s="49"/>
       <c r="J1" s="39" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="50" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
-    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
@@ -938,16 +938,16 @@
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
     </row>
-    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="58" t="s">
+      <c r="D4" s="58"/>
+      <c r="E4" s="45" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -962,7 +962,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
@@ -982,7 +982,7 @@
       <c r="H5" s="1"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>1</v>
       </c>
@@ -1001,12 +1001,12 @@
       <c r="F6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="56"/>
     </row>
-    <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
@@ -1018,8 +1018,8 @@
       <c r="I7" s="31"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="17" t="s">
         <v>15</v>
@@ -1033,7 +1033,7 @@
       <c r="I9" s="18"/>
       <c r="J9" s="19"/>
     </row>
-    <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="20" t="s">
         <v>25</v>
@@ -1051,7 +1051,7 @@
       <c r="I10" s="24"/>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="20" t="s">
         <v>18</v>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="J11" s="25"/>
     </row>
-    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>

</xml_diff>

<commit_message>
Fix: broader column template + removed string transformations for product category + replace underscore with space (product area)
</commit_message>
<xml_diff>
--- a/templates/packlista_template.xlsx
+++ b/templates/packlista_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\Jupyter\Enterprise\SvenskaKyrkan\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0513B83-B9EA-44CB-B199-5F3343279126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9E1824-3CD1-4654-B436-00937BDE8798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,7 +870,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +880,7 @@
     <col min="3" max="3" width="6.140625" style="36" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" style="36" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="36" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="36" customWidth="1"/>
     <col min="7" max="7" width="5.28515625" style="36" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" style="36" customWidth="1"/>
     <col min="9" max="9" width="6.7109375" style="36" customWidth="1"/>

</xml_diff>

<commit_message>
Switch for pask or jul Top-aligned detail cell in template
</commit_message>
<xml_diff>
--- a/templates/packlista_template.xlsx
+++ b/templates/packlista_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\JupyterLab\Kyrkan\WebShopReport\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0392BB13-BC19-4E16-BAC1-1D3A08CCA255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC451D42-87D3-46F3-801C-C69EDEE510D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -147,7 +147,7 @@
     <numFmt numFmtId="165" formatCode="hh:mm;@"/>
     <numFmt numFmtId="166" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -452,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1"/>
@@ -515,9 +515,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -526,43 +523,44 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -873,10 +871,10 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="33" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="33" customWidth="1"/>
@@ -891,69 +889,69 @@
     <col min="11" max="11" width="13.140625" style="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.45" customHeight="1">
-      <c r="A1" s="50"/>
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="42"/>
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="34"/>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="52"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="53"/>
+      <c r="K1"/>
     </row>
-    <row r="2" spans="1:11" ht="58.5" customHeight="1">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="46" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="53"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
+      <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A3" s="56"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="53"/>
+    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" ht="27.75" customHeight="1">
+    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="40" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -967,10 +965,10 @@
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="53"/>
+      <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1">
-      <c r="A5" s="53"/>
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5"/>
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
@@ -988,37 +986,37 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
+      <c r="I5"/>
+      <c r="J5"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="45" customHeight="1">
+    <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14">
         <v>1</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="38">
         <v>11</v>
       </c>
       <c r="F6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="47"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="53"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A7" s="59"/>
+    <row r="7" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
       <c r="B7" s="26"/>
       <c r="C7" s="27"/>
       <c r="D7" s="28"/>
@@ -1028,22 +1026,22 @@
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
-      <c r="K7" s="53"/>
+      <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
+    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1">
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="16" t="s">
         <v>21</v>
@@ -1056,9 +1054,9 @@
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
       <c r="J9" s="18"/>
-      <c r="K9" s="53"/>
+      <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" ht="21.6" customHeight="1">
+    <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="19" t="s">
         <v>22</v>
@@ -1075,9 +1073,9 @@
       <c r="H10" s="22"/>
       <c r="I10" s="23"/>
       <c r="J10" s="25"/>
-      <c r="K10" s="53"/>
+      <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" ht="21.6" customHeight="1">
+    <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="19" t="s">
         <v>25</v>
@@ -1096,9 +1094,9 @@
         <v>28</v>
       </c>
       <c r="J11" s="24"/>
-      <c r="K11" s="53"/>
+      <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1">
+    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1109,7 +1107,7 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="53"/>
+      <c r="K12"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>